<commit_message>
InputSAP - adding info into Help tab
InputSAP - adding info into Help tab
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carvaa/Projects/ProposalCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/ProposalCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -120,9 +120,6 @@
     <t>31/01/2017</t>
   </si>
   <si>
-    <t>standard</t>
-  </si>
-  <si>
     <t>Partial Upfront</t>
   </si>
   <si>
@@ -144,15 +141,6 @@
     <t>Linux</t>
   </si>
   <si>
-    <t>SQL Server Enterprise</t>
-  </si>
-  <si>
-    <t>SQL Std</t>
-  </si>
-  <si>
-    <t>SQL Web</t>
-  </si>
-  <si>
     <t>Server 1</t>
   </si>
   <si>
@@ -213,10 +201,82 @@
     <t>Apps</t>
   </si>
   <si>
-    <t>HANA OLTP</t>
-  </si>
-  <si>
     <t>S3 Backup(GB)</t>
+  </si>
+  <si>
+    <t>US East (Ohio)</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>APPS</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>US West (Oregon)</t>
+  </si>
+  <si>
+    <t>Convertible</t>
+  </si>
+  <si>
+    <t>ANY_DB</t>
+  </si>
+  <si>
+    <t>SQLStandard</t>
+  </si>
+  <si>
+    <t>US West (N. California)</t>
+  </si>
+  <si>
+    <t>HANA_OLTP</t>
+  </si>
+  <si>
+    <t>SQLWeb</t>
+  </si>
+  <si>
+    <t>HANA_OLAP</t>
+  </si>
+  <si>
+    <t>SQLEnterprise</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Mumbai)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Seoul)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Singapore)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Sydney)</t>
+  </si>
+  <si>
+    <t>Asia Pacific (Tokyo)</t>
+  </si>
+  <si>
+    <t>AWS GovCloud (US)</t>
+  </si>
+  <si>
+    <t>Canada (Central)</t>
+  </si>
+  <si>
+    <t>China (Beijing)</t>
+  </si>
+  <si>
+    <t>EU (Frankfurt)</t>
+  </si>
+  <si>
+    <t>EU (Ireland)</t>
+  </si>
+  <si>
+    <t>EU (London)</t>
+  </si>
+  <si>
+    <t>Valid Combinations for Purchasing Option</t>
   </si>
 </sst>
 </file>
@@ -226,10 +286,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -287,16 +354,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -304,26 +390,186 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1123,9 +1369,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G1:S6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="G1:S6"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="G1:T17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="G1:T17"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="Storage(GB)" dataDxfId="16"/>
     <tableColumn id="2" name="Volume Type" dataDxfId="15"/>
     <tableColumn id="3" name="IOPS"/>
@@ -1136,6 +1382,7 @@
     <tableColumn id="8" name="Offering Class" dataDxfId="11"/>
     <tableColumn id="9" name="Tenancy" dataDxfId="10"/>
     <tableColumn id="10" name="Operating System"/>
+    <tableColumn id="14" name="SAP Instance Type"/>
     <tableColumn id="11" name="Pre Installed S/W"/>
     <tableColumn id="12" name="Beginning" dataDxfId="9"/>
     <tableColumn id="13" name="End" dataDxfId="8"/>
@@ -1145,8 +1392,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table5" displayName="Table5" ref="A1:F17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Description" dataDxfId="5"/>
     <tableColumn id="2" name="Region" dataDxfId="4"/>
@@ -1424,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,16 +1706,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -1498,10 +1745,10 @@
         <v>17</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>9</v>
@@ -1521,13 +1768,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>20</v>
@@ -1569,18 +1816,18 @@
         <v>24</v>
       </c>
       <c r="U2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -1622,18 +1869,18 @@
         <v>24</v>
       </c>
       <c r="U3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
@@ -1675,18 +1922,18 @@
         <v>24</v>
       </c>
       <c r="U4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>20</v>
@@ -1728,18 +1975,18 @@
         <v>24</v>
       </c>
       <c r="U5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>20</v>
@@ -1781,18 +2028,18 @@
         <v>24</v>
       </c>
       <c r="U6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
@@ -1837,7 +2084,7 @@
         <v>24</v>
       </c>
       <c r="U7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1851,18 +2098,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
@@ -1881,7 +2128,7 @@
     <col min="20" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1931,21 +2178,24 @@
         <v>12</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1975,13 +2225,13 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>11</v>
@@ -1990,18 +2240,21 @@
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -2013,7 +2266,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -2022,100 +2275,361 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
       </c>
       <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
         <v>31</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P4" t="s">
         <v>34</v>
       </c>
-      <c r="P3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G4" s="2">
-        <v>100</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>35</v>
-      </c>
       <c r="Q4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="R4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G5" s="2">
         <v>500</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="G6" s="2">
         <v>500</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="Q7"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="P8"/>
       <c r="Q8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="P9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q9"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q10"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="P11"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q11"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="P12"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q12"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="P13"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q13"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="P14"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q14"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="P15"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q15"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="P16"/>
-    </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="Q16"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="13"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="I24" s="31"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="I26" s="31"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="I28" s="31"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="R29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Creating comboboxes for input_sap
Creating comboboxes for input_sap
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
   <si>
     <t>Description</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Archive Logs/Local Backup(GB)</t>
   </si>
   <si>
-    <t>Apps</t>
-  </si>
-  <si>
     <t>S3 Backup(GB)</t>
   </si>
   <si>
@@ -277,6 +274,15 @@
   </si>
   <si>
     <t>Valid Combinations for Purchasing Option</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>partial Upfront</t>
+  </si>
+  <si>
+    <t>uS East (N. Virginia)</t>
   </si>
 </sst>
 </file>
@@ -536,15 +542,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +567,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1339,8 +1345,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U1048575" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="A1:U1048575"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U1048576" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="A1:U1048576"/>
   <tableColumns count="21">
     <tableColumn id="1" name="Description" dataDxfId="39"/>
     <tableColumn id="2" name="Environment" dataDxfId="38"/>
@@ -1669,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1748,7 +1754,7 @@
         <v>55</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>9</v>
@@ -1774,7 +1780,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>20</v>
@@ -1803,19 +1809,19 @@
       <c r="P2" s="2">
         <v>100</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1827,10 +1833,10 @@
         <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E3" s="2">
         <v>4000</v>
@@ -1857,19 +1863,19 @@
         <v>100</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
         <v>24</v>
       </c>
       <c r="U3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -1880,10 +1886,10 @@
         <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E4" s="2">
         <v>8000</v>
@@ -1891,9 +1897,6 @@
       <c r="G4" s="9">
         <v>0.1</v>
       </c>
-      <c r="I4" s="9">
-        <v>0.05</v>
-      </c>
       <c r="J4" s="2">
         <v>100</v>
       </c>
@@ -1910,16 +1913,16 @@
         <v>100</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="S4" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="T4" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="U4" t="s">
         <v>35</v>
@@ -1933,16 +1936,13 @@
         <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="2">
         <v>20</v>
-      </c>
-      <c r="E5" s="2">
-        <v>16000</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0.1</v>
       </c>
       <c r="I5" s="9">
         <v>0.05</v>
@@ -1963,19 +1963,19 @@
         <v>100</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S5" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="T5" t="s">
         <v>24</v>
       </c>
       <c r="U5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1986,10 +1986,10 @@
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2">
         <v>32000</v>
@@ -2016,7 +2016,7 @@
         <v>100</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>22</v>
@@ -2025,10 +2025,10 @@
         <v>23</v>
       </c>
       <c r="T6" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="U6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -2039,10 +2039,10 @@
         <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2">
         <v>72000</v>
@@ -2072,20 +2072,27 @@
         <v>100</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="S7" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
       </c>
       <c r="U7" t="s">
-        <v>35</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="1"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2093,6 +2100,54 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$Q$2:$Q$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$B$2:$B$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$M$2:$M$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>S2:S300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$N$2:$N$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>T2:T300</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$P$2:$P$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U300</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2100,7 +2155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -2195,7 +2250,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -2231,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>11</v>
@@ -2240,10 +2295,10 @@
         <v>28</v>
       </c>
       <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
         <v>60</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>29</v>
@@ -2254,7 +2309,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -2284,7 +2339,7 @@
         <v>30</v>
       </c>
       <c r="N3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
@@ -2293,15 +2348,15 @@
         <v>35</v>
       </c>
       <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R3" t="s">
         <v>64</v>
-      </c>
-      <c r="R3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="2">
         <v>100</v>
@@ -2316,10 +2371,10 @@
         <v>34</v>
       </c>
       <c r="Q4" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" t="s">
         <v>67</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -2336,15 +2391,15 @@
         <v>36</v>
       </c>
       <c r="Q5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" t="s">
         <v>69</v>
-      </c>
-      <c r="R5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2">
         <v>500</v>
@@ -2356,13 +2411,13 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R7"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P8"/>
       <c r="Q8"/>
@@ -2370,7 +2425,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -2378,7 +2433,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P10"/>
       <c r="Q10"/>
@@ -2386,7 +2441,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P11"/>
       <c r="Q11"/>
@@ -2394,7 +2449,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P12"/>
       <c r="Q12"/>
@@ -2402,7 +2457,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P13"/>
       <c r="Q13"/>
@@ -2410,7 +2465,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P14"/>
       <c r="Q14"/>
@@ -2418,7 +2473,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P15"/>
       <c r="Q15"/>
@@ -2426,7 +2481,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P16"/>
       <c r="Q16"/>
@@ -2444,185 +2499,185 @@
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="21" t="s">
-        <v>59</v>
+      <c r="D22" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>59</v>
+      <c r="D23" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="I24" s="31"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
+      <c r="D24" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="I24" s="28"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>59</v>
+      <c r="D25" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="I26" s="31"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
+      <c r="D26" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+      <c r="I26" s="28"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="34" t="s">
-        <v>63</v>
+      <c r="D27" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:18" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
-      <c r="I28" s="31"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
+      <c r="D28" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+      <c r="I28" s="28"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="38" t="s">
-        <v>63</v>
+      <c r="D29" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="R29" s="1"/>
     </row>

</xml_diff>

<commit_message>
Removing invalid storage types
Removing invalid storage types for SAP workloads
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carvaa/Projects/ProposalCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/ProposalCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
   <si>
     <t>Description</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Monthly Utilization</t>
   </si>
   <si>
-    <t>Magnetic</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
@@ -136,12 +133,6 @@
   </si>
   <si>
     <t>General Purpose</t>
-  </si>
-  <si>
-    <t>Throughput Optimized HDD</t>
-  </si>
-  <si>
-    <t>Cold HDD</t>
   </si>
   <si>
     <t>OnDemand</t>
@@ -1497,7 +1488,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1528,16 +1519,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -1567,27 +1558,27 @@
         <v>15</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
@@ -1611,7 +1602,7 @@
         <v>100</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N2" s="2">
         <v>100</v>
@@ -1623,21 +1614,21 @@
         <v>100</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -1661,7 +1652,7 @@
         <v>200</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="2">
         <v>200</v>
@@ -1673,23 +1664,23 @@
         <v>100</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S3"/>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
@@ -1713,7 +1704,7 @@
         <v>300</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N4" s="2">
         <v>300</v>
@@ -1725,21 +1716,21 @@
         <v>100</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -1763,7 +1754,7 @@
         <v>400</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="2">
         <v>400</v>
@@ -1775,21 +1766,21 @@
         <v>100</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
@@ -1813,7 +1804,7 @@
         <v>500</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N6" s="2">
         <v>500</v>
@@ -1825,21 +1816,21 @@
         <v>100</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1863,7 +1854,7 @@
         <v>600</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="2">
         <v>600</v>
@@ -1875,21 +1866,21 @@
         <v>100</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1913,7 +1904,7 @@
         <v>700</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N8" s="2">
         <v>700</v>
@@ -1925,21 +1916,21 @@
         <v>100</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -1963,7 +1954,7 @@
         <v>800</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" s="2">
         <v>800</v>
@@ -1975,21 +1966,21 @@
         <v>100</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -2013,7 +2004,7 @@
         <v>900</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" s="2">
         <v>900</v>
@@ -2025,10 +2016,10 @@
         <v>100</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2078,15 +2069,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$I$2:$I$6</xm:f>
+            <xm:f>Help!$S$2:$S$10</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>R2:R1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$S$2:$S$10</xm:f>
+            <xm:f>Help!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2099,7 +2090,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2131,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>6</v>
@@ -2179,21 +2170,21 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="S1" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -2210,8 +2201,8 @@
       <c r="H2" s="4">
         <v>100</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="J2" s="4">
         <v>5</v>
@@ -2223,33 +2214,33 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
@@ -2261,7 +2252,7 @@
         <v>100</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3">
         <v>1000</v>
@@ -2270,54 +2261,51 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" s="2">
         <v>100</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -2327,116 +2315,110 @@
       <c r="H5" s="2">
         <v>500</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="Q5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H6" s="2">
         <v>500</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="S6" s="19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q8"/>
       <c r="R8"/>
       <c r="S8" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Q11"/>
       <c r="R11"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q12"/>
       <c r="R12"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Q13"/>
       <c r="R13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q17"/>
       <c r="R17"/>

</xml_diff>

<commit_message>
adding new Billing Option: 3YNU
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Server 9</t>
+  </si>
+  <si>
+    <t>3 Yr No Upfront Reserved</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -435,9 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2084,7 +2084,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$S$2:$S$10</xm:f>
+            <xm:f>Help!$S$2:$S$11</xm:f>
           </x14:formula1>
           <xm:sqref>R2:R1048576</xm:sqref>
         </x14:dataValidation>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2181,7 @@
       <c r="R1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2351,15 +2351,15 @@
         <v>37</v>
       </c>
       <c r="S6" s="19" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>78</v>
+      <c r="S7" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -2368,8 +2368,8 @@
       </c>
       <c r="Q8"/>
       <c r="R8"/>
-      <c r="S8" s="19" t="s">
-        <v>79</v>
+      <c r="S8" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -2378,8 +2378,8 @@
       </c>
       <c r="Q9"/>
       <c r="R9"/>
-      <c r="S9" s="2" t="s">
-        <v>80</v>
+      <c r="S9" s="20" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -2388,8 +2388,8 @@
       </c>
       <c r="Q10"/>
       <c r="R10"/>
-      <c r="S10" s="21" t="s">
-        <v>81</v>
+      <c r="S10" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -2398,6 +2398,9 @@
       </c>
       <c r="Q11"/>
       <c r="R11"/>
+      <c r="S11" s="20" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">

</xml_diff>

<commit_message>
BYOL sap instances and standby instances
BYOL sap instances and standby instances
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>SUSE</t>
   </si>
   <si>
-    <t>Linux</t>
-  </si>
-  <si>
     <t>Server 1</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Memory(GB)</t>
+  </si>
+  <si>
+    <t>BYOL</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1187,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R1048576" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="A1:R1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:R1048574" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="A1:R1048574"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Description" dataDxfId="36"/>
     <tableColumn id="2" name="Environment" dataDxfId="35"/>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,16 +1547,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>1</v>
@@ -1565,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>5</v>
@@ -1586,27 +1586,27 @@
         <v>15</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
@@ -1630,7 +1630,7 @@
         <v>1000.5</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="22">
         <v>2000.5</v>
@@ -1645,18 +1645,18 @@
         <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -1680,7 +1680,7 @@
         <v>200</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="22">
         <v>200</v>
@@ -1695,20 +1695,20 @@
         <v>29</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S3"/>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
@@ -1732,7 +1732,7 @@
         <v>300</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="22">
         <v>300</v>
@@ -1747,18 +1747,18 @@
         <v>29</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -1782,7 +1782,7 @@
         <v>400</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5" s="22">
         <v>400</v>
@@ -1797,18 +1797,18 @@
         <v>29</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
@@ -1832,7 +1832,7 @@
         <v>500</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="22">
         <v>500</v>
@@ -1847,18 +1847,18 @@
         <v>29</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1882,7 +1882,7 @@
         <v>500</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="22">
         <v>500</v>
@@ -1897,18 +1897,18 @@
         <v>29</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1932,7 +1932,7 @@
         <v>600</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="22">
         <v>600</v>
@@ -1947,18 +1947,18 @@
         <v>29</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -1982,7 +1982,7 @@
         <v>700</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="22">
         <v>700</v>
@@ -1997,18 +1997,18 @@
         <v>29</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -2032,7 +2032,7 @@
         <v>800</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N10" s="22">
         <v>800</v>
@@ -2047,18 +2047,18 @@
         <v>29</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -2082,7 +2082,7 @@
         <v>900</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N11" s="22">
         <v>900</v>
@@ -2097,7 +2097,7 @@
         <v>29</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2109,12 +2109,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Help!$C$2:$C$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D300</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$N$2:$N$4</xm:f>
@@ -2129,33 +2123,39 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Help!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D298</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Help!$Q$2:$Q$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q300</xm:sqref>
+          <xm:sqref>Q2:Q298</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B2:B1048574</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$S$2:$S$11</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>R2:R1048574</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:L1048576</xm:sqref>
+          <xm:sqref>L1:L1048574</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Help!$R$2:$R$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>C2:C1048574</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2167,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>6</v>
@@ -2248,21 +2248,21 @@
         <v>10</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -2280,7 +2280,7 @@
         <v>100</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="4">
         <v>5</v>
@@ -2298,7 +2298,7 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>9</v>
@@ -2307,18 +2307,18 @@
         <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
@@ -2330,7 +2330,7 @@
         <v>100</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3">
         <v>1000</v>
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
@@ -2348,7 +2348,7 @@
         <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" t="s">
         <v>27</v>
@@ -2357,18 +2357,18 @@
         <v>29</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="2">
         <v>100</v>
@@ -2380,10 +2380,10 @@
         <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -2394,115 +2394,115 @@
         <v>500</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="R5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="2">
         <v>500</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q8"/>
       <c r="R8"/>
       <c r="S8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q12"/>
       <c r="R12"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q13"/>
       <c r="R13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q17"/>
       <c r="R17"/>

</xml_diff>

<commit_message>
Environment changes in the input_sap.xlsx
Environment changes in the input_sap.xlsx
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -286,12 +286,33 @@
   </si>
   <si>
     <t>BYOL</t>
+  </si>
+  <si>
+    <t>HA</t>
+  </si>
+  <si>
+    <t>SANDBOX</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>NON_PROD</t>
+  </si>
+  <si>
+    <t>DR_FULL</t>
+  </si>
+  <si>
+    <t>DR_OPTIMIZED</t>
+  </si>
+  <si>
+    <t>DR_INACTIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1515,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2135,7 +2156,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Help!$B$2:$B$4</xm:f>
+            <xm:f>Help!$B$2:$B$11</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048574</xm:sqref>
         </x14:dataValidation>
@@ -2167,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2387,6 +2408,9 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
@@ -2404,6 +2428,9 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2418,6 +2445,9 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
@@ -2426,6 +2456,9 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>58</v>
       </c>
@@ -2436,6 +2469,9 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>59</v>
       </c>
@@ -2446,6 +2482,9 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
@@ -2456,6 +2495,9 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>61</v>
       </c>
@@ -2557,6 +2599,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Removing China and adding Paris
Removing China and adding Paris region
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -219,9 +219,6 @@
     <t>Canada (Central)</t>
   </si>
   <si>
-    <t>China (Beijing)</t>
-  </si>
-  <si>
     <t>EU (Frankfurt)</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>DR_INACTIVE</t>
+  </si>
+  <si>
+    <t>EU (Paris)</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1537,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1586,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>5</v>
@@ -1616,7 +1616,7 @@
         <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1666,12 +1666,12 @@
         <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>44</v>
@@ -1716,7 +1716,7 @@
         <v>29</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S3"/>
       <c r="T3"/>
@@ -1768,7 +1768,7 @@
         <v>29</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
         <v>29</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -1868,7 +1868,7 @@
         <v>29</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -1918,12 +1918,12 @@
         <v>29</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>44</v>
@@ -1968,12 +1968,12 @@
         <v>29</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>44</v>
@@ -2018,12 +2018,12 @@
         <v>29</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>44</v>
@@ -2068,12 +2068,12 @@
         <v>29</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>44</v>
@@ -2118,7 +2118,7 @@
         <v>29</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2141,12 +2141,6 @@
             <xm:f>Help!$O$2:$O$3</xm:f>
           </x14:formula1>
           <xm:sqref>T3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Help!$C$2:$C$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D298</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2178,6 +2172,12 @@
           </x14:formula1>
           <xm:sqref>C2:C1048574</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Help!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048574</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2189,7 +2189,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2272,7 +2272,7 @@
         <v>42</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -2331,7 +2331,7 @@
         <v>49</v>
       </c>
       <c r="S2" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>52</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -2404,12 +2404,12 @@
         <v>54</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
@@ -2418,18 +2418,18 @@
         <v>500</v>
       </c>
       <c r="Q5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R5" t="s">
         <v>55</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>56</v>
@@ -2438,26 +2438,26 @@
         <v>500</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S6" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>58</v>
@@ -2465,12 +2465,12 @@
       <c r="Q8"/>
       <c r="R8"/>
       <c r="S8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>59</v>
@@ -2478,12 +2478,12 @@
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>60</v>
@@ -2491,12 +2491,12 @@
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>61</v>
@@ -2504,7 +2504,7 @@
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="Q16"/>
       <c r="R16"/>

</xml_diff>

<commit_message>
EFS Pricing - Parameters tab
</commit_message>
<xml_diff>
--- a/input_sap.xlsx
+++ b/input_sap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravanini/WorkDocs/workspace/SapSizerCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757657AA-4378-AF45-9FDE-914E785EBDBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30770E-3C0B-7449-880A-170D12DF6D04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" xr2:uid="{6D211BAE-D26B-E74A-B969-920951E188BB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13900" activeTab="1" xr2:uid="{6D211BAE-D26B-E74A-B969-920951E188BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>US West (Los Angeles)</t>
+  </si>
+  <si>
+    <t>Elastic File System (in GB)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2AC007D-B14B-A842-9703-8D72B01CF1C1}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -969,19 +972,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6535EF-9F0E-F043-A0F3-3C3FAFE713F7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -991,8 +995,11 @@
       <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
@@ -1001,6 +1008,9 @@
       </c>
       <c r="C2" s="6" t="s">
         <v>67</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>